<commit_message>
Added DataProvider logic for parameterization.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krishnasakinala/eclipse-workspace1/POM_HybridFramework_Java/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E39D25-FDB3-F042-AA3E-DCAC6B43114C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144BACA2-8DF4-1948-ADBF-C49B9F2EE83C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,7 +99,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -202,21 +202,6 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -238,9 +223,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,7 +509,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,10 +519,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
@@ -549,7 +534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -561,8 +546,8 @@
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="20" x14ac:dyDescent="0.25">
@@ -581,7 +566,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -593,8 +578,8 @@
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>10</v>
+      <c r="B8" s="8" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>